<commit_message>
evil in the detail
</commit_message>
<xml_diff>
--- a/统计.xlsx
+++ b/统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2E4BB2-7500-4603-88F2-F14F191454DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1206153-4CE9-4B74-A688-AF04F754C741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5270C8F1-6B76-463D-9211-2891EA8507AB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -93,6 +93,10 @@
   </si>
   <si>
     <t>74双</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75双</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -239,12 +243,119 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61双</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62双</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63双</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64双</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65双</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66双</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>70双</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>71双</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>73双</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>74双</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>75双</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>287</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$32</c:f>
+              <c:f>Sheet1!$B$2:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -337,6 +448,12 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -367,6 +484,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -594,12 +712,119 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$34</c:f>
+              <c:strCache>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>258</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61双</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62双</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>262</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>63双</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>263</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>264</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64双</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>65双</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>267</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>268</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66双</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>269</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>70双</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>277</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>278</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>71双</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>282</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>73双</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>284</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>74双</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>285</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>286</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>75双</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>287</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$32</c:f>
+              <c:f>Sheet1!$E$2:$E$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="33"/>
                 <c:pt idx="0">
                   <c:v>0.76875414914804163</c:v>
                 </c:pt>
@@ -692,6 +917,12 @@
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0.10099337748344371</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.1414071510957324</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.14594039054470709</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -722,7 +953,8 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
+        <c:numFmt formatCode="#,##0_);\(#,##0\)" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -744,6 +976,9 @@
           <a:p>
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1995,8 +2230,8 @@
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
@@ -2031,8 +2266,8 @@
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
@@ -2359,10 +2594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7176F916-26A8-4C45-9EC2-0E9253DB5856}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2416,7 +2651,7 @@
         <v>2534</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E32" si="0">C3/D3</f>
+        <f t="shared" ref="E3:E34" si="0">C3/D3</f>
         <v>0.23717442778216258</v>
       </c>
     </row>
@@ -2940,6 +3175,42 @@
       <c r="E32">
         <f t="shared" si="0"/>
         <v>0.10099337748344371</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>613</v>
+      </c>
+      <c r="D33">
+        <v>4335</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>0.1414071510957324</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>287</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>994</v>
+      </c>
+      <c r="D34">
+        <v>6811</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="0"/>
+        <v>0.14594039054470709</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
well done for me
</commit_message>
<xml_diff>
--- a/统计.xlsx
+++ b/统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1206153-4CE9-4B74-A688-AF04F754C741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E1EC9E-11DB-4FAC-9645-2BB70B75DA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5270C8F1-6B76-463D-9211-2891EA8507AB}"/>
   </bookViews>
@@ -245,9 +245,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$34</c:f>
+              <c:f>Sheet1!$A$2:$A$35</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>258</c:v>
                 </c:pt>
@@ -346,16 +346,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>287</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>290</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$34</c:f>
+              <c:f>Sheet1!$B$2:$B$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -453,6 +456,9 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -714,9 +720,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$34</c:f>
+              <c:f>Sheet1!$A$2:$A$35</c:f>
               <c:strCache>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>258</c:v>
                 </c:pt>
@@ -815,16 +821,19 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>287</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>290</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$34</c:f>
+              <c:f>Sheet1!$E$2:$E$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="33"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
                   <c:v>0.76875414914804163</c:v>
                 </c:pt>
@@ -923,6 +932,9 @@
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0.14594039054470709</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.4741035856573712E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2594,10 +2606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7176F916-26A8-4C45-9EC2-0E9253DB5856}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2651,7 +2663,7 @@
         <v>2534</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E34" si="0">C3/D3</f>
+        <f t="shared" ref="E3:E35" si="0">C3/D3</f>
         <v>0.23717442778216258</v>
       </c>
     </row>
@@ -3211,6 +3223,24 @@
       <c r="E34">
         <f t="shared" si="0"/>
         <v>0.14594039054470709</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>290</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>469</v>
+      </c>
+      <c r="D35">
+        <v>6275</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="0"/>
+        <v>7.4741035856573712E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
peace of our era
</commit_message>
<xml_diff>
--- a/统计.xlsx
+++ b/统计.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22E6C24-B539-4E11-A45C-A03EFB1A7C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55821231-0191-4174-939B-BC8837333272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{5270C8F1-6B76-463D-9211-2891EA8507AB}"/>
   </bookViews>
@@ -261,9 +261,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$46</c:f>
+              <c:f>Sheet1!$A$2:$A$60</c:f>
               <c:strCache>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>258</c:v>
                 </c:pt>
@@ -398,16 +398,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>83双</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>303</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$46</c:f>
+              <c:f>Sheet1!$B$2:$B$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="59"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -541,6 +544,9 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
@@ -802,9 +808,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$46</c:f>
+              <c:f>Sheet1!$A$2:$A$60</c:f>
               <c:strCache>
-                <c:ptCount val="45"/>
+                <c:ptCount val="46"/>
                 <c:pt idx="0">
                   <c:v>258</c:v>
                 </c:pt>
@@ -939,16 +945,19 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>83双</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>303</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$46</c:f>
+              <c:f>Sheet1!$E$2:$E$60</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="45"/>
+                <c:ptCount val="59"/>
                 <c:pt idx="0">
                   <c:v>0.76875414914804163</c:v>
                 </c:pt>
@@ -1083,6 +1092,9 @@
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>0.12530989407257156</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.12087599544937429</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2756,8 +2768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7176F916-26A8-4C45-9EC2-0E9253DB5856}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2793,7 +2805,7 @@
         <v>4519</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E46" si="0">C2/D2</f>
+        <f t="shared" ref="E2:E47" si="0">C2/D2</f>
         <v>0.76875414914804163</v>
       </c>
     </row>
@@ -3592,6 +3604,19 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>303</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>850</v>
+      </c>
+      <c r="D47">
+        <v>7032</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="0"/>
+        <v>0.12087599544937429</v>
       </c>
     </row>
   </sheetData>

</xml_diff>